<commit_message>
Ok juro q n cometo mais
</commit_message>
<xml_diff>
--- a/Checklist Colorida.xlsx
+++ b/Checklist Colorida.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josphze\Desktop\SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D6932E-FEA5-46D7-9BAD-0EC85170E911}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A16588-0828-4847-8160-B30E611C2568}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -249,7 +249,7 @@
     <t>TODO do ze:</t>
   </si>
   <si>
-    <t>Yay callbacks</t>
+    <t>Podemos não estar a chamar o callback sempre q necessario</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1075,10 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1178,6 +1178,9 @@
       <c r="F9" s="14" t="s">
         <v>63</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
@@ -1276,32 +1279,26 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="10">
-        <v>3</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="12">
+        <v>3</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10">
-        <v>3</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>69</v>
+      <c r="C17" s="12">
+        <v>3</v>
       </c>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="10">
-        <v>3</v>
-      </c>
-      <c r="B18" s="11" t="s">
+      <c r="A18" s="12">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="10">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>69</v>
+      <c r="C18" s="12">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>